<commit_message>
Updating resume and covid numbers for 11/9/20
</commit_message>
<xml_diff>
--- a/data/nyc_covid_by_zcta.xlsx
+++ b/data/nyc_covid_by_zcta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbenn\Documents\Data Science\Homework_4\jthompson3175.github.io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02D1A77C-8205-48F7-95FF-2D2649D2A201}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8185FDC4-7F2F-4DD8-87FA-54E81D4458CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1259686F-3096-4824-A4F6-483968C55940}"/>
+    <workbookView xWindow="28680" yWindow="-1005" windowWidth="21840" windowHeight="13140" xr2:uid="{1259686F-3096-4824-A4F6-483968C55940}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -562,7 +562,7 @@
   <dimension ref="A1:I178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>